<commit_message>
Add sprint 0 excel sheet and fix a typo in sprint2 excel sheet
</commit_message>
<xml_diff>
--- a/Sprint2.xlsx
+++ b/Sprint2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage\homes\H8244\Dox\Desktop\GitHub\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage\homes\H8244\Dox\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,10 +35,10 @@
     <t>Kustannukset AWS-palveluista MTD</t>
   </si>
   <si>
-    <t>Tunnit yhteensä 9-1-15.1</t>
+    <t>https://github.com/DigiaMinions/Project/wiki/TUNTIKIRJAUKSET</t>
   </si>
   <si>
-    <t>https://github.com/DigiaMinions/Project/wiki/TUNTIKIRJAUKSET</t>
+    <t>Tunnit yhteensä 9.1-15.1</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>123</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2"/>
     </row>

</xml_diff>